<commit_message>
Cleaning folder, deleting unnecessary files. Renamed the Main data set and now created a "fulldata"-file with soil properties and precipitation.
In the script, the fulldata-file is created from the diffrent subdatasets. So that anychanges in the subdatasets will also change the fulldata-file
</commit_message>
<xml_diff>
--- a/Termites/Soil data/Soil_Nutrient.xlsx
+++ b/Termites/Soil data/Soil_Nutrient.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0989B0F2-A291-42B7-957C-8041B81DB6C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E9C368-4DE9-46C8-A5A7-263ECCFAE256}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="21">
   <si>
     <t>Season</t>
   </si>
@@ -147,9 +147,6 @@
   <si>
     <t>P.per (NMBU)</t>
   </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
@@ -185,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -193,26 +190,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +578,7 @@
         <v>64.81</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I59" si="0">G3/F3</f>
+        <f t="shared" ref="I3:I58" si="0">G3/F3</f>
         <v>13.071428571428571</v>
       </c>
     </row>
@@ -1006,7 +990,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1036,7 +1020,7 @@
         <v>12.647058823529409</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1050,7 @@
         <v>12.533333333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1079,7 @@
         <v>12.465034965034965</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1125,7 +1109,7 @@
         <v>13.625</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1155,7 +1139,7 @@
         <v>12.3125</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1187,13 +1171,8 @@
       <c r="J22">
         <v>0.32999999999999996</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1202,7 @@
         <v>11.555555555555555</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1256,7 +1235,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1265,7 @@
         <v>12.909090909090908</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1319,7 +1298,7 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1349,7 +1328,7 @@
         <v>12.166666666666666</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1379,7 +1358,7 @@
         <v>14.3125</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1409,7 +1388,7 @@
         <v>13.500000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1439,7 +1418,7 @@
         <v>12.428571428571427</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -1469,7 +1448,7 @@
         <v>13.769230769230768</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Corrected a "mistake". Had two values for same block in nutrient data (Handajega W2). This created to many observations in the fulldata set. So then the avarage of these two values were calculated.
</commit_message>
<xml_diff>
--- a/Termites/Soil data/Soil_Nutrient.xlsx
+++ b/Termites/Soil data/Soil_Nutrient.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E9C368-4DE9-46C8-A5A7-263ECCFAE256}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F40EDA-CE50-48C9-8D9F-6C664AFC5EC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,12 +78,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{0B4F6C3E-9DE4-476E-A81C-0F86ADB1A79E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Anders Sundsdal
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Had two results for same labeled soil. Did an avarage of these two.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G39" authorId="0" shapeId="0" xr:uid="{3ECCEC52-5732-43A3-889A-776D4D7BDC9B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Had two results for same labeled soil. Did an avarage of these two.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="21">
   <si>
     <t>Season</t>
   </si>
@@ -152,7 +200,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +220,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -477,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -578,7 +633,7 @@
         <v>64.81</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I58" si="0">G3/F3</f>
+        <f t="shared" ref="I3:I57" si="0">G3/F3</f>
         <v>13.071428571428571</v>
       </c>
     </row>
@@ -1672,17 +1727,17 @@
         <v>10</v>
       </c>
       <c r="F39">
-        <v>0.11</v>
+        <v>0.11499999999999999</v>
       </c>
       <c r="G39">
-        <v>1.52</v>
+        <v>1.56</v>
       </c>
       <c r="H39">
         <v>36.17</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>13.818181818181818</v>
+        <v>13.565217391304349</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -1696,20 +1751,23 @@
         <v>14</v>
       </c>
       <c r="D40" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
       </c>
       <c r="F40">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="G40">
-        <v>1.6</v>
+        <v>2.19</v>
+      </c>
+      <c r="H40">
+        <v>29.2</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>13.333333333333334</v>
+        <v>19.90909090909091</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -1723,23 +1781,23 @@
         <v>14</v>
       </c>
       <c r="D41" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
       </c>
       <c r="F41">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="G41">
-        <v>2.19</v>
+        <v>1.95</v>
       </c>
       <c r="H41">
-        <v>29.2</v>
+        <v>21.51</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>19.90909090909091</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -1747,29 +1805,29 @@
         <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D42" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="G42">
-        <v>1.95</v>
+        <v>1.88</v>
       </c>
       <c r="H42">
-        <v>21.51</v>
+        <v>0.86</v>
       </c>
       <c r="I42">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>12.533333333333333</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -1783,23 +1841,23 @@
         <v>15</v>
       </c>
       <c r="D43" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
       </c>
       <c r="F43">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="G43">
-        <v>1.88</v>
+        <v>2.64</v>
       </c>
       <c r="H43">
-        <v>0.86</v>
+        <v>33.11</v>
       </c>
       <c r="I43">
         <f t="shared" si="0"/>
-        <v>12.533333333333333</v>
+        <v>12.571428571428573</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -1813,23 +1871,23 @@
         <v>15</v>
       </c>
       <c r="D44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" t="s">
         <v>9</v>
       </c>
       <c r="F44">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="G44">
-        <v>2.64</v>
+        <v>3.3</v>
       </c>
       <c r="H44">
-        <v>33.11</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I44">
         <f t="shared" si="0"/>
-        <v>12.571428571428573</v>
+        <v>14.34782608695652</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -1843,23 +1901,23 @@
         <v>15</v>
       </c>
       <c r="D45" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E45" t="s">
         <v>9</v>
       </c>
       <c r="F45">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="G45">
-        <v>3.3</v>
+        <v>1.96</v>
       </c>
       <c r="H45">
-        <v>1.1000000000000001</v>
+        <v>3.05</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>14.34782608695652</v>
+        <v>13.066666666666666</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1872,24 +1930,24 @@
       <c r="C46" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="1">
-        <v>4</v>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="G46">
-        <v>1.96</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="H46">
-        <v>3.05</v>
+        <v>24.32</v>
       </c>
       <c r="I46">
         <f t="shared" si="0"/>
-        <v>13.066666666666666</v>
+        <v>12.666666666666666</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -1903,23 +1961,23 @@
         <v>15</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
       </c>
       <c r="F47">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="G47">
-        <v>2.2799999999999998</v>
+        <v>1.87</v>
       </c>
       <c r="H47">
-        <v>24.32</v>
+        <v>15.64</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
-        <v>12.666666666666666</v>
+        <v>11.6875</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -1933,23 +1991,23 @@
         <v>15</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
       </c>
       <c r="F48">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="G48">
-        <v>1.87</v>
+        <v>2.5</v>
       </c>
       <c r="H48">
-        <v>15.64</v>
+        <v>8.68</v>
       </c>
       <c r="I48">
         <f t="shared" si="0"/>
-        <v>11.6875</v>
+        <v>11.904761904761905</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -1963,23 +2021,23 @@
         <v>15</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
       </c>
       <c r="F49">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="G49">
-        <v>2.5</v>
+        <v>2.08</v>
       </c>
       <c r="H49">
-        <v>8.68</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>11.904761904761905</v>
+        <v>13.866666666666667</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -1990,26 +2048,26 @@
         <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F50">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="G50">
-        <v>2.08</v>
+        <v>2.98</v>
       </c>
       <c r="H50">
-        <v>4.1500000000000004</v>
+        <v>7.94</v>
       </c>
       <c r="I50">
         <f t="shared" si="0"/>
-        <v>13.866666666666667</v>
+        <v>15.684210526315789</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2023,23 +2081,23 @@
         <v>16</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
       </c>
       <c r="F51">
-        <v>0.19</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G51">
-        <v>2.98</v>
+        <v>3.13</v>
       </c>
       <c r="H51">
-        <v>7.94</v>
+        <v>16.739999999999998</v>
       </c>
       <c r="I51">
         <f t="shared" si="0"/>
-        <v>15.684210526315789</v>
+        <v>10.793103448275863</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2053,23 +2111,23 @@
         <v>16</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
       </c>
       <c r="F52">
-        <v>0.28999999999999998</v>
+        <v>0.18</v>
       </c>
       <c r="G52">
-        <v>3.13</v>
+        <v>2.14</v>
       </c>
       <c r="H52">
-        <v>16.739999999999998</v>
+        <v>16.5</v>
       </c>
       <c r="I52">
         <f t="shared" si="0"/>
-        <v>10.793103448275863</v>
+        <v>11.888888888888889</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2083,23 +2141,23 @@
         <v>16</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
       </c>
       <c r="F53">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="G53">
-        <v>2.14</v>
+        <v>2.35</v>
       </c>
       <c r="H53">
-        <v>16.5</v>
+        <v>22.24</v>
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
-        <v>11.888888888888889</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2107,29 +2165,29 @@
         <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F54">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="G54">
-        <v>2.35</v>
+        <v>2.95</v>
       </c>
       <c r="H54">
-        <v>22.24</v>
+        <v>61.22</v>
       </c>
       <c r="I54">
         <f t="shared" si="0"/>
-        <v>11.75</v>
+        <v>12.82608695652174</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2143,23 +2201,23 @@
         <v>11</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
         <v>11</v>
       </c>
       <c r="F55">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="G55">
-        <v>2.95</v>
+        <v>2.14</v>
       </c>
       <c r="H55">
-        <v>61.22</v>
+        <v>56.09</v>
       </c>
       <c r="I55">
         <f t="shared" si="0"/>
-        <v>12.82608695652174</v>
+        <v>14.266666666666667</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2173,23 +2231,23 @@
         <v>11</v>
       </c>
       <c r="D56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" t="s">
         <v>11</v>
       </c>
       <c r="F56">
-        <v>0.15</v>
+        <v>0.21</v>
       </c>
       <c r="G56">
-        <v>2.14</v>
+        <v>2.6</v>
       </c>
       <c r="H56">
-        <v>56.09</v>
+        <v>59.87</v>
       </c>
       <c r="I56">
         <f t="shared" si="0"/>
-        <v>14.266666666666667</v>
+        <v>12.380952380952381</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
@@ -2203,57 +2261,28 @@
         <v>11</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E57" t="s">
         <v>11</v>
       </c>
       <c r="F57">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="G57">
-        <v>2.6</v>
+        <v>2.41</v>
       </c>
       <c r="H57">
-        <v>59.87</v>
+        <v>47.26</v>
       </c>
       <c r="I57">
-        <f t="shared" si="0"/>
-        <v>12.380952380952381</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>19</v>
-      </c>
-      <c r="C58" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58">
-        <v>4</v>
-      </c>
-      <c r="E58" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58">
-        <v>0.19</v>
-      </c>
-      <c r="G58">
-        <v>2.41</v>
-      </c>
-      <c r="H58">
-        <v>47.26</v>
-      </c>
-      <c r="I58">
         <f t="shared" si="0"/>
         <v>12.684210526315789</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>